<commit_message>
Finished 1996-7 tb 3.
</commit_message>
<xml_diff>
--- a/resources/190108-pdf_manifest.xlsx
+++ b/resources/190108-pdf_manifest.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\expenditure-reports-project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85C50037-3266-4745-A819-0E4ECB8BFA08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15A0634-AFCB-4080-B0A8-2328329E35F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="181207-pdf_manifest" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'181207-pdf_manifest'!$A$1:$H$43</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Year</t>
   </si>
@@ -185,12 +193,15 @@
   </si>
   <si>
     <t>Finished</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1024,10 +1035,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1096,6 +1109,9 @@
       <c r="G3" t="s">
         <v>52</v>
       </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1142,6 +1158,9 @@
       <c r="G5" t="s">
         <v>50</v>
       </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1907,7 +1926,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H43">
+  <autoFilter ref="A1:H43" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H43">
       <sortCondition ref="A1:A43"/>
     </sortState>

</xml_diff>

<commit_message>
Working on 1999_tb3.xlsx stopped at first currency column
</commit_message>
<xml_diff>
--- a/resources/190108-pdf_manifest.xlsx
+++ b/resources/190108-pdf_manifest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\expenditure-reports-project\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudy\programming_projects\extra_curricular\expenditure-reports-project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15A0634-AFCB-4080-B0A8-2328329E35F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B53CB2E-1E1D-4355-BFAD-093ADA8B5B56}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>Year</t>
   </si>
@@ -1039,7 +1039,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,6 +1200,9 @@
       </c>
       <c r="G7" t="s">
         <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished up to 2006_tb3.xlsx. Continue with 2007_tb3
</commit_message>
<xml_diff>
--- a/resources/190108-pdf_manifest.xlsx
+++ b/resources/190108-pdf_manifest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudy\programming_projects\extra_curricular\expenditure-reports-project\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\expenditure-reports-project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B53CB2E-1E1D-4355-BFAD-093ADA8B5B56}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8FECC6-BE8D-4C23-9BED-8FC4CF201EE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>Year</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Where do other expenses come from?</t>
+  </si>
+  <si>
+    <t>Where do other expenses come from and why are only some amphibians counted in subtotal?</t>
   </si>
 </sst>
 </file>
@@ -1036,15 +1045,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1069,8 +1078,11 @@
       <c r="H1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1996</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1996</v>
       </c>
@@ -1113,7 +1125,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1997</v>
       </c>
@@ -1136,7 +1148,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1997</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1998</v>
       </c>
@@ -1182,7 +1194,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1998</v>
       </c>
@@ -1205,7 +1217,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1999</v>
       </c>
@@ -1225,7 +1237,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1999</v>
       </c>
@@ -1244,8 +1256,11 @@
       <c r="G9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2000</v>
       </c>
@@ -1265,7 +1280,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2000</v>
       </c>
@@ -1284,8 +1299,11 @@
       <c r="G11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2001</v>
       </c>
@@ -1305,7 +1323,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2001</v>
       </c>
@@ -1324,8 +1342,14 @@
       <c r="G13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -1345,7 +1369,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2002</v>
       </c>
@@ -1364,8 +1388,14 @@
       <c r="G15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1385,7 +1415,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -1404,8 +1434,14 @@
       <c r="G17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2004</v>
       </c>
@@ -1425,7 +1461,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2004</v>
       </c>
@@ -1444,8 +1480,14 @@
       <c r="G19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2005</v>
       </c>
@@ -1465,7 +1507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2005</v>
       </c>
@@ -1484,8 +1526,14 @@
       <c r="G21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2006</v>
       </c>
@@ -1505,7 +1553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2006</v>
       </c>
@@ -1524,8 +1572,14 @@
       <c r="G23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2007</v>
       </c>
@@ -1545,7 +1599,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2007</v>
       </c>
@@ -1565,7 +1619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2008</v>
       </c>
@@ -1585,7 +1639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2008</v>
       </c>
@@ -1605,7 +1659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2009</v>
       </c>
@@ -1625,7 +1679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2009</v>
       </c>
@@ -1645,7 +1699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2010</v>
       </c>
@@ -1665,7 +1719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2010</v>
       </c>
@@ -1685,7 +1739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2011</v>
       </c>

</xml_diff>

<commit_message>
Extracted 2009-10 using Java Tabula. Continue with cleaning these csvs.
</commit_message>
<xml_diff>
--- a/resources/190108-pdf_manifest.xlsx
+++ b/resources/190108-pdf_manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\expenditure-reports-project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8FECC6-BE8D-4C23-9BED-8FC4CF201EE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9E8354-752B-4A68-9350-146954DD09A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
   <si>
     <t>Year</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Where do other expenses come from and why are only some amphibians counted in subtotal?</t>
+  </si>
+  <si>
+    <t>Mammals subtotal is inconsistent</t>
+  </si>
+  <si>
+    <t>Working on cleaning up</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,6 +1624,12 @@
       <c r="G25" t="s">
         <v>28</v>
       </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1658,6 +1670,12 @@
       <c r="G27" t="s">
         <v>26</v>
       </c>
+      <c r="H27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1698,6 +1716,9 @@
       <c r="G29" t="s">
         <v>24</v>
       </c>
+      <c r="I29" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1737,6 +1758,9 @@
       </c>
       <c r="G31" t="s">
         <v>22</v>
+      </c>
+      <c r="I31" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Continue working on 1996_tb2.xlsx on page 10 of the PDF
</commit_message>
<xml_diff>
--- a/resources/190108-pdf_manifest.xlsx
+++ b/resources/190108-pdf_manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\expenditure-reports-project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9E8354-752B-4A68-9350-146954DD09A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A68012-84BA-43B3-BC83-3FFB14772F2C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t>Year</t>
   </si>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,6 +1716,9 @@
       <c r="G29" t="s">
         <v>24</v>
       </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
       <c r="I29" t="s">
         <v>59</v>
       </c>
@@ -1759,6 +1762,9 @@
       <c r="G31" t="s">
         <v>22</v>
       </c>
+      <c r="H31" t="s">
+        <v>54</v>
+      </c>
       <c r="I31" t="s">
         <v>59</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -1802,8 +1808,11 @@
       <c r="G33" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2012</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2012</v>
       </c>
@@ -1842,8 +1851,11 @@
       <c r="G35" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2013</v>
       </c>
@@ -1863,7 +1875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2013</v>
       </c>
@@ -1882,8 +1894,11 @@
       <c r="G37" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2014</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2014</v>
       </c>
@@ -1922,8 +1937,11 @@
       <c r="G39" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2015</v>
       </c>
@@ -1943,7 +1961,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2015</v>
       </c>
@@ -1962,8 +1980,11 @@
       <c r="G41" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2016</v>
       </c>
@@ -1986,7 +2007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2016</v>
       </c>
@@ -2004,6 +2025,9 @@
       </c>
       <c r="G43" t="s">
         <v>10</v>
+      </c>
+      <c r="H43" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>